<commit_message>
Cập nhật .Net 8. Thao tác Đọc - Ghi - Sửa - Xóa dữ liệu từ file excel
</commit_message>
<xml_diff>
--- a/WebMVC/Datas/ds_sinhvien.xlsx
+++ b/WebMVC/Datas/ds_sinhvien.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>tt</t>
   </si>
@@ -48,10 +48,16 @@
     <t>dienthoai</t>
   </si>
   <si>
+    <t>diem_tichluy</t>
+  </si>
+  <si>
     <t>diem_renluyen</t>
   </si>
   <si>
-    <t>diem_tichluy</t>
+    <t>xet_hocbong</t>
+  </si>
+  <si>
+    <t>1112</t>
   </si>
   <si>
     <t>Nguyen Thi</t>
@@ -60,83 +66,36 @@
     <t>Hai</t>
   </si>
   <si>
-    <t>Tran Van</t>
-  </si>
-  <si>
-    <t>Thanh</t>
+    <t>haint</t>
+  </si>
+  <si>
+    <t>haint@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>0988111111</t>
+  </si>
+  <si>
+    <t>Dang Thai</t>
   </si>
   <si>
     <t>Chau</t>
   </si>
   <si>
-    <t>Hoang Hai</t>
-  </si>
-  <si>
-    <t>Nam</t>
-  </si>
-  <si>
-    <t>Dinh Manh</t>
-  </si>
-  <si>
-    <t>Thang</t>
-  </si>
-  <si>
-    <t>Dang Thai</t>
-  </si>
-  <si>
-    <t>haint</t>
-  </si>
-  <si>
-    <t>thanhtv</t>
-  </si>
-  <si>
     <t>chaudt</t>
   </si>
   <si>
-    <t>thangdm</t>
-  </si>
-  <si>
-    <t>namhn</t>
-  </si>
-  <si>
-    <t>haint@vnuf.edu.vn</t>
-  </si>
-  <si>
-    <t>thanhtv@vnuf.edu.vn</t>
-  </si>
-  <si>
     <t>chaudt@vnuf.edu.vn</t>
   </si>
   <si>
-    <t>namhn@vnuf.edu.vn</t>
-  </si>
-  <si>
-    <t>thangdm@vnuf.edu.vn</t>
-  </si>
-  <si>
-    <t>0988111111</t>
-  </si>
-  <si>
-    <t>0978222222</t>
-  </si>
-  <si>
     <t>0966333333</t>
-  </si>
-  <si>
-    <t>0912444444</t>
-  </si>
-  <si>
-    <t>0923555555</t>
-  </si>
-  <si>
-    <t>xet_hocbong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,7 +126,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J1048576"/>
@@ -461,188 +420,102 @@
     <col min="6" max="6" width="20.77734375" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="14.6640625" customWidth="1"/>
     <col min="10" max="10" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="0">
+        <v>2.2</v>
+      </c>
+      <c r="I2" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0">
+        <v>333</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>222</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3">
-        <v>2.8</v>
-      </c>
-      <c r="I3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>333</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4">
+      <c r="H3" s="0">
         <v>4</v>
       </c>
-      <c r="I4">
+      <c r="I3" s="0">
         <v>6.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>444</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5">
-        <v>1.6</v>
-      </c>
-      <c r="I5">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>555</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Viết API Get All Student, Get Student by ID
</commit_message>
<xml_diff>
--- a/WebMVC/Datas/ds_sinhvien.xlsx
+++ b/WebMVC/Datas/ds_sinhvien.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoatx\source\repos\67IT-ASP.NET\WebMVC\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoatx\source\repos\67IT-ASP.NET\BT3\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CD457B-E8C8-45A8-B538-96AE5DF75574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FB48F9-B08B-4D70-B042-CDB7950451B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>tt</t>
   </si>
@@ -48,54 +48,92 @@
     <t>dienthoai</t>
   </si>
   <si>
+    <t>diem_renluyen</t>
+  </si>
+  <si>
     <t>diem_tichluy</t>
   </si>
   <si>
-    <t>diem_renluyen</t>
-  </si>
-  <si>
-    <t>xet_hocbong</t>
-  </si>
-  <si>
-    <t>1112</t>
-  </si>
-  <si>
     <t>Nguyen Thi</t>
   </si>
   <si>
     <t>Hai</t>
   </si>
   <si>
+    <t>Tran Van</t>
+  </si>
+  <si>
+    <t>Thanh</t>
+  </si>
+  <si>
+    <t>Chau</t>
+  </si>
+  <si>
+    <t>Hoang Hai</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Dinh Manh</t>
+  </si>
+  <si>
+    <t>Thang</t>
+  </si>
+  <si>
+    <t>Dang Thai</t>
+  </si>
+  <si>
     <t>haint</t>
   </si>
   <si>
+    <t>thanhtv</t>
+  </si>
+  <si>
+    <t>chaudt</t>
+  </si>
+  <si>
+    <t>thangdm</t>
+  </si>
+  <si>
+    <t>namhn</t>
+  </si>
+  <si>
     <t>haint@vnuf.edu.vn</t>
   </si>
   <si>
+    <t>thanhtv@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>chaudt@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>namhn@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>thangdm@vnuf.edu.vn</t>
+  </si>
+  <si>
     <t>0988111111</t>
   </si>
   <si>
-    <t>Dang Thai</t>
-  </si>
-  <si>
-    <t>Chau</t>
-  </si>
-  <si>
-    <t>chaudt</t>
-  </si>
-  <si>
-    <t>chaudt@vnuf.edu.vn</t>
+    <t>0978222222</t>
   </si>
   <si>
     <t>0966333333</t>
+  </si>
+  <si>
+    <t>0912444444</t>
+  </si>
+  <si>
+    <t>0923555555</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,7 +164,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,102 +458,184 @@
     <col min="6" max="6" width="20.77734375" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" bestFit="1" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="0" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>222</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>2.8</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>333</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>444</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="0">
-        <v>2.2</v>
-      </c>
-      <c r="I2" s="0">
-        <v>10</v>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5">
+        <v>1.6</v>
+      </c>
+      <c r="I5">
+        <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0">
-        <v>333</v>
-      </c>
-      <c r="C3" s="0" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>555</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="0">
-        <v>4</v>
-      </c>
-      <c r="I3" s="0">
-        <v>6.5</v>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update thao tác thêm mới, sửa, xóa bằng JS và call API
</commit_message>
<xml_diff>
--- a/WebMVC/Datas/ds_sinhvien.xlsx
+++ b/WebMVC/Datas/ds_sinhvien.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>tt</t>
   </si>
@@ -48,92 +48,126 @@
     <t>dienthoai</t>
   </si>
   <si>
+    <t>diem_tichluy</t>
+  </si>
+  <si>
     <t>diem_renluyen</t>
   </si>
   <si>
-    <t>diem_tichluy</t>
-  </si>
-  <si>
     <t>Nguyen Thi</t>
   </si>
   <si>
     <t>Hai</t>
   </si>
   <si>
+    <t>haint</t>
+  </si>
+  <si>
+    <t>haint@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>0988111111</t>
+  </si>
+  <si>
     <t>Tran Van</t>
   </si>
   <si>
     <t>Thanh</t>
   </si>
   <si>
+    <t>thanhtv</t>
+  </si>
+  <si>
+    <t>thanhtv@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>0978222222</t>
+  </si>
+  <si>
+    <t>Dang Thai</t>
+  </si>
+  <si>
     <t>Chau</t>
   </si>
   <si>
+    <t>chaudt</t>
+  </si>
+  <si>
+    <t>chaudt@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>0966333333</t>
+  </si>
+  <si>
     <t>Hoang Hai</t>
   </si>
   <si>
     <t>Nam</t>
   </si>
   <si>
+    <t>namhn</t>
+  </si>
+  <si>
+    <t>namhn@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>0912444444</t>
+  </si>
+  <si>
     <t>Dinh Manh</t>
   </si>
   <si>
     <t>Thang</t>
   </si>
   <si>
-    <t>Dang Thai</t>
-  </si>
-  <si>
-    <t>haint</t>
-  </si>
-  <si>
-    <t>thanhtv</t>
-  </si>
-  <si>
-    <t>chaudt</t>
-  </si>
-  <si>
     <t>thangdm</t>
   </si>
   <si>
-    <t>namhn</t>
-  </si>
-  <si>
-    <t>haint@vnuf.edu.vn</t>
-  </si>
-  <si>
-    <t>thanhtv@vnuf.edu.vn</t>
-  </si>
-  <si>
-    <t>chaudt@vnuf.edu.vn</t>
-  </si>
-  <si>
-    <t>namhn@vnuf.edu.vn</t>
-  </si>
-  <si>
     <t>thangdm@vnuf.edu.vn</t>
   </si>
   <si>
-    <t>0988111111</t>
-  </si>
-  <si>
-    <t>0978222222</t>
-  </si>
-  <si>
-    <t>0966333333</t>
-  </si>
-  <si>
-    <t>0912444444</t>
-  </si>
-  <si>
     <t>0923555555</t>
+  </si>
+  <si>
+    <t>2233444</t>
+  </si>
+  <si>
+    <t>Giang</t>
+  </si>
+  <si>
+    <t>namgiang</t>
+  </si>
+  <si>
+    <t>namgiang@gmail.com</t>
+  </si>
+  <si>
+    <t>234224</t>
+  </si>
+  <si>
+    <t>6454</t>
+  </si>
+  <si>
+    <t>Trần Văn</t>
+  </si>
+  <si>
+    <t>An</t>
+  </si>
+  <si>
+    <t>antv</t>
+  </si>
+  <si>
+    <t>antv@gmail.com</t>
+  </si>
+  <si>
+    <t>34455345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,7 +198,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -458,184 +492,243 @@
     <col min="6" max="6" width="20.77734375" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0">
+        <v>111</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="0">
+        <v>2.2</v>
+      </c>
+      <c r="I2" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0">
+        <v>222</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="0">
+        <v>2.8</v>
+      </c>
+      <c r="I3" s="0">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0">
+        <v>333</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="0">
+        <v>4</v>
+      </c>
+      <c r="I4" s="0">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0">
+        <v>444</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="D5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="0">
+        <v>1.6</v>
+      </c>
+      <c r="I5" s="0">
+        <v>8.8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0">
+        <v>555</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="H2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>222</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="D6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H3">
-        <v>2.8</v>
-      </c>
-      <c r="I3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>333</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="E6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>444</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="F6" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="H5">
-        <v>1.6</v>
-      </c>
-      <c r="I5">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>555</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="0">
+        <v>3</v>
+      </c>
+      <c r="I7" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="0">
+        <v>4</v>
+      </c>
+      <c r="I8" s="0">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật API PUT (đủ các trường dữ liệu). Xử lý Frontend JS chỉnh sửa và call api cập nhật
</commit_message>
<xml_diff>
--- a/WebMVC/Datas/ds_sinhvien.xlsx
+++ b/WebMVC/Datas/ds_sinhvien.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>tt</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>diem_renluyen</t>
+  </si>
+  <si>
+    <t>11123</t>
   </si>
   <si>
     <t>Nguyen Thi</t>
@@ -528,23 +531,23 @@
       <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" s="0">
-        <v>111</v>
+      <c r="B2" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0">
         <v>2.2</v>
@@ -561,19 +564,19 @@
         <v>222</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="0">
         <v>2.8</v>
@@ -590,19 +593,19 @@
         <v>333</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="0">
         <v>4</v>
@@ -619,19 +622,19 @@
         <v>444</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H5" s="0">
         <v>1.6</v>
@@ -648,19 +651,19 @@
         <v>555</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H6" s="0">
         <v>2</v>
@@ -674,22 +677,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" s="0">
         <v>3</v>
@@ -703,22 +706,22 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8" s="0">
         <v>4</v>

</xml_diff>

<commit_message>
Có thể thay thế bằng hàm pop() để lấy về phần tử cuối cùng của array
</commit_message>
<xml_diff>
--- a/WebMVC/Datas/ds_sinhvien.xlsx
+++ b/WebMVC/Datas/ds_sinhvien.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>tt</t>
   </si>
@@ -54,22 +54,19 @@
     <t>diem_renluyen</t>
   </si>
   <si>
-    <t>11123</t>
-  </si>
-  <si>
-    <t>Nguyen Thi</t>
-  </si>
-  <si>
-    <t>Hai</t>
-  </si>
-  <si>
-    <t>haint</t>
-  </si>
-  <si>
-    <t>haint@vnuf.edu.vn</t>
-  </si>
-  <si>
-    <t>0988111111</t>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>Hoàng</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>nam_abc</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
   <si>
     <t>Tran Van</t>
@@ -103,9 +100,6 @@
   </si>
   <si>
     <t>Hoang Hai</t>
-  </si>
-  <si>
-    <t>Nam</t>
   </si>
   <si>
     <t>namhn</t>
@@ -547,13 +541,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="0">
-        <v>2.2</v>
+        <v>4</v>
       </c>
       <c r="I2" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -564,19 +558,19 @@
         <v>222</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="H3" s="0">
         <v>2.8</v>
@@ -593,19 +587,19 @@
         <v>333</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="H4" s="0">
         <v>4</v>
@@ -622,19 +616,19 @@
         <v>444</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="H5" s="0">
         <v>1.6</v>
@@ -651,19 +645,19 @@
         <v>555</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="H6" s="0">
         <v>2</v>
@@ -677,22 +671,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="H7" s="0">
         <v>3</v>
@@ -706,22 +700,22 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="H8" s="0">
         <v>4</v>

</xml_diff>

<commit_message>
Một trường hợp ví dụ thực hiện sắp xếp, xử lý trên Frontend
</commit_message>
<xml_diff>
--- a/WebMVC/Datas/ds_sinhvien.xlsx
+++ b/WebMVC/Datas/ds_sinhvien.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>tt</t>
   </si>
@@ -63,10 +63,13 @@
     <t>Nam</t>
   </si>
   <si>
-    <t>nam_abc</t>
-  </si>
-  <si>
-    <t>string</t>
+    <t>nam_abc_xyz</t>
+  </si>
+  <si>
+    <t>nam_abc_xyz@gmail.com</t>
+  </si>
+  <si>
+    <t>tỷyryrty</t>
   </si>
   <si>
     <t>Tran Van</t>
@@ -124,39 +127,6 @@
   </si>
   <si>
     <t>0923555555</t>
-  </si>
-  <si>
-    <t>2233444</t>
-  </si>
-  <si>
-    <t>Giang</t>
-  </si>
-  <si>
-    <t>namgiang</t>
-  </si>
-  <si>
-    <t>namgiang@gmail.com</t>
-  </si>
-  <si>
-    <t>234224</t>
-  </si>
-  <si>
-    <t>6454</t>
-  </si>
-  <si>
-    <t>Trần Văn</t>
-  </si>
-  <si>
-    <t>An</t>
-  </si>
-  <si>
-    <t>antv</t>
-  </si>
-  <si>
-    <t>antv@gmail.com</t>
-  </si>
-  <si>
-    <t>34455345</t>
   </si>
 </sst>
 </file>
@@ -476,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -541,7 +511,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0">
         <v>4</v>
@@ -558,19 +528,19 @@
         <v>222</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="0">
         <v>2.8</v>
@@ -587,19 +557,19 @@
         <v>333</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="0">
         <v>4</v>
@@ -616,19 +586,19 @@
         <v>444</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" s="0">
         <v>1.6</v>
@@ -645,83 +615,25 @@
         <v>555</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="0">
         <v>2</v>
       </c>
       <c r="I6" s="0">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="0">
-        <v>3</v>
-      </c>
-      <c r="I7" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0">
-        <v>8</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="0">
-        <v>4</v>
-      </c>
-      <c r="I8" s="0">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cập nhật sắp xếp tăng dần giảm dần, tùy biến theo trường. Và thêm API sort để sắp xếp nếu gọi API
</commit_message>
<xml_diff>
--- a/WebMVC/Datas/ds_sinhvien.xlsx
+++ b/WebMVC/Datas/ds_sinhvien.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>tt</t>
   </si>
@@ -60,49 +60,52 @@
     <t>Hoàng</t>
   </si>
   <si>
+    <t>Giang</t>
+  </si>
+  <si>
+    <t>nam_abc_xyz</t>
+  </si>
+  <si>
+    <t>nam_abc_xyz@gmail.com</t>
+  </si>
+  <si>
+    <t>tỷyryrty</t>
+  </si>
+  <si>
+    <t>Tran Van</t>
+  </si>
+  <si>
+    <t>Thanh</t>
+  </si>
+  <si>
+    <t>thanhtv</t>
+  </si>
+  <si>
+    <t>thanhtv@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>0978222222</t>
+  </si>
+  <si>
+    <t>Dang Thai</t>
+  </si>
+  <si>
+    <t>Chau</t>
+  </si>
+  <si>
+    <t>chaudt</t>
+  </si>
+  <si>
+    <t>chaudt@vnuf.edu.vn</t>
+  </si>
+  <si>
+    <t>0966333333</t>
+  </si>
+  <si>
+    <t>Hoang Hai</t>
+  </si>
+  <si>
     <t>Nam</t>
-  </si>
-  <si>
-    <t>nam_abc_xyz</t>
-  </si>
-  <si>
-    <t>nam_abc_xyz@gmail.com</t>
-  </si>
-  <si>
-    <t>tỷyryrty</t>
-  </si>
-  <si>
-    <t>Tran Van</t>
-  </si>
-  <si>
-    <t>Thanh</t>
-  </si>
-  <si>
-    <t>thanhtv</t>
-  </si>
-  <si>
-    <t>thanhtv@vnuf.edu.vn</t>
-  </si>
-  <si>
-    <t>0978222222</t>
-  </si>
-  <si>
-    <t>Dang Thai</t>
-  </si>
-  <si>
-    <t>Chau</t>
-  </si>
-  <si>
-    <t>chaudt</t>
-  </si>
-  <si>
-    <t>chaudt@vnuf.edu.vn</t>
-  </si>
-  <si>
-    <t>0966333333</t>
-  </si>
-  <si>
-    <t>Hoang Hai</t>
   </si>
   <si>
     <t>namhn</t>
@@ -589,16 +592,16 @@
         <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H5" s="0">
         <v>1.6</v>
@@ -615,19 +618,19 @@
         <v>555</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H6" s="0">
         <v>2</v>

</xml_diff>